<commit_message>
last update before test
last update before test
</commit_message>
<xml_diff>
--- a/DarkGameProject/Assets/Resources/Excel/gameTask.xlsx
+++ b/DarkGameProject/Assets/Resources/Excel/gameTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kanjess/Desktop/MP_DarkGame/DarkGameProject/Assets/Resources/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033BA7C5-0C3C-1D47-9CBC-ED553DF4C9BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8E7C4F-DBDF-AF4B-ADC6-0CCF511D520E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{340A7935-8C9A-6041-96F0-1FEBE449ED49}"/>
   </bookViews>
@@ -1330,7 +1330,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t> the arrow from &lt;color=green&gt;App Store&lt;/color&gt; module to the &lt;color=blue&gt;Basic Function or Gameplay&lt;/color&gt; module you want to connect with.</t>
+      <t> the arrow from &lt;color=#0ca300&gt;App Store&lt;/color&gt; module to the &lt;color=blue&gt;Basic Function or Gameplay&lt;/color&gt; module you want to connect with.</t>
     </r>
   </si>
 </sst>
@@ -1759,7 +1759,7 @@
   <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3219,8 +3219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16164BD-4F47-8D4D-9FCD-E64BA0FDF780}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="107" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>